<commit_message>
Changed method locators() + imported new libraries
</commit_message>
<xml_diff>
--- a/excel/alloptions.xlsx
+++ b/excel/alloptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\PycharmProjects\Testing-tool\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359B87B1-164B-4E0D-AA83-5A7A3A6A9B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D07C59B-14E4-4E40-BB31-832781F6F8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Browser</t>
   </si>
@@ -73,6 +73,48 @@
   </si>
   <si>
     <t>Must be after search</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>Clear string in search box</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Check if title matches with input string</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Waiting  for some time(in seconds)</t>
+  </si>
+  <si>
+    <t>A1:Specification of step A2:Which browser shoud be used</t>
+  </si>
+  <si>
+    <t>(Chrome, Firefox, Safari, Edge)</t>
+  </si>
+  <si>
+    <t>Inputs:</t>
+  </si>
+  <si>
+    <t>B1: Specification of step B2: Input of URL</t>
+  </si>
+  <si>
+    <t>Anything on web</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -390,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +447,7 @@
     <col min="5" max="5" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +472,14 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -450,8 +498,14 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -459,17 +513,104 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
         <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>